<commit_message>
foglio coclea du robe
</commit_message>
<xml_diff>
--- a/FogliCalcolo/Coclea/Coclea.xlsx
+++ b/FogliCalcolo/Coclea/Coclea.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\Coclea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\Coclea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AC216E-91C5-48B9-BA3D-6C9D2699FC6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A22C4F-5687-42F4-B7F0-9F1E84115927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3885" windowWidth="21600" windowHeight="11385" xr2:uid="{9673A59A-D298-4A4C-A537-28E68921EDCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9673A59A-D298-4A4C-A537-28E68921EDCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Design1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="51">
   <si>
     <t>Q</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Dati</t>
-  </si>
-  <si>
-    <t>coeff riempimento</t>
   </si>
   <si>
     <t>coeff pendenza</t>
@@ -238,6 +235,12 @@
   </si>
   <si>
     <t>Leff</t>
+  </si>
+  <si>
+    <t>coeff riempimento (in funz del materiale)</t>
+  </si>
+  <si>
+    <t>lunghezza troncone coclea</t>
   </si>
 </sst>
 </file>
@@ -468,6 +471,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,14 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -813,24 +816,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94BAE0A-8159-45C5-ACCE-6B91B37B7B6D}">
   <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -844,12 +847,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -878,13 +881,13 @@
     </row>
     <row r="5" spans="2:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>650</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="1" t="s">
@@ -910,7 +913,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -935,7 +938,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>26</v>
@@ -968,7 +971,7 @@
     </row>
     <row r="9" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="16">
         <f>C3*240/(3.6*C6*C7*C5*PI())</f>
@@ -979,10 +982,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
@@ -1004,15 +1007,15 @@
         <v>0.1</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" ref="C11:C21" si="0">$C$9/(B11^3)</f>
+        <f>$C$9/(B11^3)</f>
         <v>15960.8375978197</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="36" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4">
@@ -1028,13 +1031,13 @@
         <v>0.15</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C11:C21" si="0">$C$9/(B12^3)</f>
         <v>4729.137066020653</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="33"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="14">
         <f>(I10/C3*60-TRUNC(I10/C3*60))*60</f>
         <v>54.545454545454604</v>
@@ -1141,37 +1144,39 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="25"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="35">
+      <c r="B24" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="28">
         <v>3500</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="B25" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="35">
+      <c r="C25" s="28">
         <f>_xlfn.CEILING.MATH(C4*1000/C24)</f>
         <v>3</v>
       </c>
@@ -1179,10 +1184,10 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="35">
+      <c r="B26" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="28">
         <f>C24*C25/1000</f>
         <v>10.5</v>
       </c>
@@ -1200,7 +1205,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -1210,9 +1215,9 @@
       <c r="C28" s="2">
         <v>0.8</v>
       </c>
-      <c r="D28" s="36"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -1276,10 +1281,10 @@
     </row>
     <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
     </row>
@@ -1298,14 +1303,14 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="5">
         <f>C21*B21/60</f>
         <v>0.73892766656572706</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="3"/>
     </row>
@@ -1340,24 +1345,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178C56C0-394B-4C0F-8E57-1F85ECB67C53}">
   <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -1371,12 +1376,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1405,13 +1410,13 @@
     </row>
     <row r="5" spans="2:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>650</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="1" t="s">
@@ -1437,7 +1442,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -1462,7 +1467,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>26</v>
@@ -1495,7 +1500,7 @@
     </row>
     <row r="9" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="16">
         <f>C3*240/(3.6*C6*C7*C5*PI())</f>
@@ -1506,10 +1511,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
@@ -1536,10 +1541,10 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="36" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4">
@@ -1560,8 +1565,8 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="33"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="14">
         <f>(I10/C3*60-TRUNC(I10/C3*60))*60</f>
         <v>0</v>
@@ -1668,53 +1673,55 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="35">
+      <c r="B24" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="28">
         <v>3500</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B25" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="37"/>
-    </row>
-    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="35">
+      <c r="C25" s="28">
         <f>_xlfn.CEILING.MATH(C4*1000/C24)</f>
         <v>3</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="37"/>
+      <c r="E25" s="30"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="35">
+      <c r="B26" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="28">
         <f>C24*C25/1000</f>
         <v>10.5</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="30"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1725,7 +1732,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1737,7 +1744,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1801,10 +1808,10 @@
     </row>
     <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
     </row>
@@ -1823,14 +1830,14 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="5">
         <f>C21*B21/60</f>
         <v>0.3948259146028375</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="3"/>
     </row>
@@ -1865,24 +1872,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F445C9BA-8079-4DF4-9721-D0B0A04C9A74}">
   <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -1896,12 +1903,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -1930,13 +1937,13 @@
     </row>
     <row r="5" spans="2:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2">
         <v>650</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3"/>
       <c r="G5" s="1" t="s">
@@ -1962,7 +1969,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -1987,7 +1994,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>26</v>
@@ -2020,7 +2027,7 @@
     </row>
     <row r="9" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="16">
         <f>C3*240/(3.6*C6*C7*C5*PI())</f>
@@ -2031,10 +2038,10 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
@@ -2061,10 +2068,10 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="36" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4">
@@ -2085,8 +2092,8 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="33"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="14">
         <f>(I10/C3*60-TRUNC(I10/C3*60))*60</f>
         <v>0</v>
@@ -2194,35 +2201,37 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="35">
+      <c r="B24" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="28">
         <v>3500</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B25" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="35">
+      <c r="C25" s="28">
         <f>_xlfn.CEILING.MATH(C4*1000/C24)</f>
         <v>3</v>
       </c>
@@ -2230,10 +2239,10 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="35">
+      <c r="B26" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="28">
         <f>C24*C25/1000</f>
         <v>10.5</v>
       </c>
@@ -2251,7 +2260,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -2263,7 +2272,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -2327,10 +2336,10 @@
     </row>
     <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="12"/>
       <c r="E35" s="13"/>
     </row>
@@ -2349,14 +2358,14 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" s="5">
         <f>C21*B21/60</f>
         <v>0.13435048483013218</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="3"/>
     </row>

</xml_diff>